<commit_message>
Update files to create timetable
</commit_message>
<xml_diff>
--- a/assets/data/timetable/school_timetables_with_room.xlsx
+++ b/assets/data/timetable/school_timetables_with_room.xlsx
@@ -430,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,16 @@
           <t>Lesson 5</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -473,27 +483,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Math - Room 107</t>
+          <t>Литература - Room 105 - Teacher: Владимир В.П.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Language - Room 206</t>
+          <t>Русский язык - Room 205 - Teacher: Екатерина А.П.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Language - Room 208</t>
+          <t>Физика - Room 110 - Teacher: Роман А.Д.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Language - Room 206</t>
+          <t>Математика - Room 205 - Teacher: Евгения О.П.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Math - Room 108</t>
+          <t>Математика - Room 108 - Teacher: Алексей С.К.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Математика - Room 205 - Teacher: Константин В.Л.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>География - Room 109 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
     </row>
@@ -505,27 +525,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Math - Room 108</t>
+          <t>Физика - Room 114 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Math - Room 100</t>
+          <t>Информатика - Room 107 - Teacher: Анастасия А.М.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Language - Room 202</t>
+          <t>Физика - Room 113 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Иностранный язык - Room 207 - Teacher: Елена В.К.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Русский язык - Room 213 - Teacher: Александр И.Р.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Химия - Room 211 - Teacher: Оксана М.С.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Физическая культура - Room 111 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
     </row>
@@ -537,27 +567,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Физическая культура - Room 112 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Math - Room 101</t>
+          <t>Обществознание - Room 213 - Teacher: Наталья Д.З.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Русский язык - Room 108 - Teacher: Ольга В.С.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Информатика - Room 107 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Chemistry - Room 209</t>
+          <t>Химия - Room 211 - Teacher: Елена С.Т.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Математика - Room 205 - Teacher: Игорь П.В.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>История - Room 114 - Teacher: Елена В.К.</t>
         </is>
       </c>
     </row>
@@ -569,27 +609,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Chemistry - Room 209</t>
+          <t>Обществознание - Room 214 - Teacher: Наталья Д.З.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Биология - Room 309 - Teacher: Андрей П.С.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>История - Room 111 - Teacher: Елена В.К.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Math - Room 101</t>
+          <t>Математика - Room 109 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Physics - Room 112</t>
+          <t>География - Room 109 - Teacher: Василий И.М.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Литература - Room 202 - Teacher: Мария А.К.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Алёна В.Л.</t>
         </is>
       </c>
     </row>
@@ -601,27 +651,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Math - Room 105</t>
+          <t>Русский язык - Room 206 - Teacher: Анна С.И.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>History - Room 318</t>
+          <t>Математика - Room 109 - Teacher: Игорь П.В.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Geography - Room 316</t>
+          <t>Иностранный язык - Room 203 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Language - Room 203</t>
+          <t>X - Room 0 - Teacher: X</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Physics - Room 112</t>
+          <t>Литература - Room 207 - Teacher: Светлана А.К.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Химия - Room 212 - Teacher: Анастасия А.Ф.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Биология - Room 309 - Teacher: Светлана А.К.</t>
         </is>
       </c>
     </row>
@@ -636,7 +696,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -670,6 +730,16 @@
           <t>Lesson 5</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -679,27 +749,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Language - Room 203</t>
+          <t>Информатика - Room 107 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Geography - Room 316</t>
+          <t>Русский язык - Room 110 - Teacher: Анна С.И.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Math - Room 107</t>
+          <t>Иностранный язык - Room 203 - Teacher: Елена В.К.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Биология - Room 309 - Teacher: Андрей П.С.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>История - Room 114 - Teacher: Елена В.К.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>X - Room 0 - Teacher: X</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Химия - Room 211 - Teacher: Анастасия А.Ф.</t>
         </is>
       </c>
     </row>
@@ -711,27 +791,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Math - Room 105</t>
+          <t>Физическая культура - Room 112 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Математика - Room 212 - Teacher: Игорь П.В.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Language - Room 204</t>
+          <t>Информатика - Room 107 - Teacher: Алёна В.Л.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Русский язык - Room 101 - Teacher: Екатерина А.П.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Language - Room 208</t>
+          <t>География - Room 109 - Teacher: Василий И.М.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Русский язык - Room 213 - Teacher: Екатерина А.П.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Математика - Room 104 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
     </row>
@@ -743,27 +833,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Biology - Room 310</t>
+          <t>Физика - Room 113 - Teacher: Роман А.Д.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Language - Room 200</t>
+          <t>Обществознание - Room 212 - Teacher: Наталья Д.З.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Math - Room 101</t>
+          <t>История - Room 110 - Teacher: Елена В.К.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Литература - Room 103 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Chemistry - Room 210</t>
+          <t>Литература - Room 202 - Teacher: Илья В.М.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Математика - Room 205 - Teacher: Константин В.Л.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Физика - Room 110 - Teacher: Людмила А.С.</t>
         </is>
       </c>
     </row>
@@ -775,27 +875,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Math - Room 108</t>
+          <t>Математика - Room 212 - Teacher: Сергей А.Т.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Physics - Room 113</t>
+          <t>Физическая культура - Room 112 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Physics - Room 112</t>
+          <t>Химия - Room 209 - Teacher: Елена С.Т.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Math - Room 107</t>
+          <t>Математика - Room 205 - Teacher: Игорь П.В.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>History - Room 318</t>
+          <t>Физика - Room 114 - Teacher: Игорь В.Н.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Обществознание - Room 212 - Teacher: Анна С.И.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
     </row>
@@ -807,27 +917,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Русский язык - Room 110 - Teacher: Александр И.Р.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Language - Room 203</t>
+          <t>Математика - Room 205 - Teacher: Сергей А.Т.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Math - Room 106</t>
+          <t>Литература - Room 209 - Teacher: Георгий Н.М.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Math - Room 106</t>
+          <t>Иностранный язык - Room 206 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Chemistry - Room 210</t>
+          <t>Химия - Room 212 - Teacher: Оксана М.С.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Биология - Room 310 - Teacher: Андрей П.С.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>География - Room 109 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
     </row>
@@ -842,7 +962,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,6 +996,16 @@
           <t>Lesson 5</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -885,27 +1015,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Физическая культура - Room 112 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Math - Room 104</t>
+          <t>Русский язык - Room 206 - Teacher: Александр И.Р.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Math - Room 108</t>
+          <t>Математика - Room 212 - Teacher: Сергей А.Т.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Физика - Room 113 - Teacher: Роман А.Д.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Chemistry - Room 209</t>
+          <t>Русский язык - Room 213 - Teacher: Михаил С.К.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Математика - Room 205 - Teacher: Игорь П.В.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Иностранный язык - Room 203 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
     </row>
@@ -917,27 +1057,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Language - Room 205</t>
+          <t>Биология - Room 309 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Math - Room 104</t>
+          <t>Русский язык - Room 213 - Teacher: Михаил С.К.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Language - Room 208</t>
+          <t>Литература - Room 105 - Teacher: Илья В.М.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Physics - Room 112</t>
+          <t>История - Room 110 - Teacher: Елена В.К.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Geography - Room 315</t>
+          <t>Информатика - Room 107 - Teacher: Игорь В.Н.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Химия - Room 213 - Teacher: Елена С.Т.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Физика - Room 113 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
     </row>
@@ -949,27 +1099,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Математика - Room 109 - Teacher: Константин В.Л.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Math - Room 102</t>
+          <t>Обществознание - Room 214 - Teacher: Анна С.И.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Language - Room 203</t>
+          <t>Биология - Room 309 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Language - Room 204</t>
+          <t>Русский язык - Room 206 - Teacher: Ольга В.С.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Biology - Room 310</t>
+          <t>Иностранный язык - Room 206 - Teacher: Елена В.К.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>География - Room 109 - Teacher: Василий И.М.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>X - Room 0 - Teacher: X</t>
         </is>
       </c>
     </row>
@@ -981,27 +1141,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Math - Room 108</t>
+          <t>Физическая культура - Room 111 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Math - Room 101</t>
+          <t>Математика - Room 205 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Physics - Room 114</t>
+          <t>Обществознание - Room 214 - Teacher: Анна С.И.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Language - Room 205</t>
+          <t>Математика - Room 108 - Teacher: Евгения О.П.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Language - Room 201</t>
+          <t>Литература - Room 105 - Teacher: Петр И.С.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>История - Room 111 - Teacher: Наталья Д.З.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Химия - Room 213 - Teacher: Анастасия А.Ф.</t>
         </is>
       </c>
     </row>
@@ -1013,27 +1183,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Math - Room 103</t>
+          <t>География - Room 109 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Chemistry - Room 209</t>
+          <t>Математика - Room 205 - Teacher: Константин В.Л.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Химия - Room 212 - Teacher: Оксана М.С.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Литература - Room 212 - Teacher: Георгий Н.М.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>History - Room 319</t>
+          <t>Физика - Room 110 - Teacher: Роман А.Д.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Анастасия А.М.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Анастасия А.М.</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1228,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1082,6 +1262,16 @@
           <t>Lesson 5</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1091,27 +1281,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Математика - Room 101 - Teacher: Евгения О.П.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Математика - Room 205 - Teacher: Алексей С.К.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Math - Room 100</t>
+          <t>История - Room 114 - Teacher: Елена В.К.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Chemistry - Room 211</t>
+          <t>Обществознание - Room 213 - Teacher: Наталья Д.З.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Math - Room 102</t>
+          <t>Математика - Room 212 - Teacher: Марина Г.Б.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Физическая культура - Room 111 - Teacher: Светлана А.К.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Русский язык - Room 101 - Teacher: Михаил С.К.</t>
         </is>
       </c>
     </row>
@@ -1123,27 +1323,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Physics - Room 110</t>
+          <t>Физическая культура - Room 111 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Русский язык - Room 101 - Teacher: Екатерина А.П.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Math - Room 101</t>
+          <t>X - Room 0 - Teacher: X</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Language - Room 205</t>
+          <t>Иностранный язык - Room 206 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Math - Room 100</t>
+          <t>Обществознание - Room 212 - Teacher: Наталья Д.З.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Физика - Room 110 - Teacher: Роман А.Д.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Иностранный язык - Room 206 - Teacher: Елена В.К.</t>
         </is>
       </c>
     </row>
@@ -1155,27 +1365,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Math - Room 108</t>
+          <t>Литература - Room 202 - Teacher: Илья В.М.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Физика - Room 110 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Химия - Room 211 - Teacher: Елена С.Т.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Language - Room 200</t>
+          <t>География - Room 109 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Language - Room 204</t>
+          <t>Математика - Room 109 - Teacher: Алексей С.К.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Биология - Room 310 - Teacher: Андрей П.С.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Химия - Room 212 - Teacher: Оксана М.С.</t>
         </is>
       </c>
     </row>
@@ -1187,27 +1407,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Информатика - Room 107 - Teacher: Алёна В.Л.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>History - Room 318</t>
+          <t>Литература - Room 202 - Teacher: Владимир В.П.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Language - Room 206</t>
+          <t>История - Room 111 - Teacher: Елена В.К.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Химия - Room 209 - Teacher: Елена С.Т.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Литература - Room 207 - Teacher: Владимир В.П.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Алёна В.Л.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>География - Room 111 - Teacher: Василий И.М.</t>
         </is>
       </c>
     </row>
@@ -1219,27 +1449,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Physics - Room 111</t>
+          <t>Биология - Room 310 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Geography - Room 316</t>
+          <t>Физика - Room 111 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Chemistry - Room 211</t>
+          <t>Русский язык - Room 213 - Teacher: Александр И.Р.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Math - Room 104</t>
+          <t>Математика - Room 109 - Teacher: Сергей А.Т.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Math - Room 105</t>
+          <t>Русский язык - Room 110 - Teacher: Анна С.И.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Математика - Room 109 - Teacher: Константин В.Л.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Алёна В.Л.</t>
         </is>
       </c>
     </row>
@@ -1254,7 +1494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1288,6 +1528,16 @@
           <t>Lesson 5</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1297,27 +1547,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Обществознание - Room 214 - Teacher: Анна С.И.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Math - Room 107</t>
+          <t>Литература - Room 210 - Teacher: Владимир В.П.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Language - Room 208</t>
+          <t>Информатика - Room 107 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Chemistry - Room 209</t>
+          <t>Русский язык - Room 101 - Teacher: Дмитрий А.Ф.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Math - Room 108</t>
+          <t>Литература - Room 202 - Teacher: Владимир В.П.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Иностранный язык - Room 206 - Teacher: Елена В.К.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
     </row>
@@ -1329,27 +1589,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Language - Room 201</t>
+          <t>Математика - Room 104 - Teacher: Алексей С.К.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Math - Room 104</t>
+          <t>Математика - Room 212 - Teacher: Евгения О.П.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Language - Room 203</t>
+          <t>Иностранный язык - Room 208 - Teacher: Елена В.К.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Math - Room 103</t>
+          <t>Математика - Room 109 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Math - Room 100</t>
+          <t>Химия - Room 213 - Teacher: Оксана М.С.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>История - Room 111 - Teacher: Наталья Д.З.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Математика - Room 109 - Teacher: Евгения О.П.</t>
         </is>
       </c>
     </row>
@@ -1361,27 +1631,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Language - Room 205</t>
+          <t>Биология - Room 310 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Математика - Room 109 - Teacher: Евгения О.П.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Chemistry - Room 210</t>
+          <t>Русский язык - Room 206 - Teacher: Михаил С.К.</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Русский язык - Room 213 - Teacher: Дмитрий А.Ф.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Physics - Room 111</t>
+          <t>География - Room 111 - Teacher: Марина Г.Б.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Физика - Room 114 - Teacher: Роман А.Д.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Математика - Room 205 - Teacher: Евгения О.П.</t>
         </is>
       </c>
     </row>
@@ -1393,27 +1673,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Math - Room 107</t>
+          <t>X - Room 0 - Teacher: X</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Language - Room 206</t>
+          <t>Обществознание - Room 214 - Teacher: Анна С.И.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Физическая культура - Room 112 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>History - Room 318</t>
+          <t>Физическая культура - Room 112 - Teacher: Юлия Н.В.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Physics - Room 109</t>
+          <t>Литература - Room 202 - Teacher: Илья В.М.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Химия - Room 211 - Teacher: Оксана М.С.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Анастасия А.М.</t>
         </is>
       </c>
     </row>
@@ -1425,27 +1715,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Физика - Room 114 - Teacher: Роман А.Д.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Math - Room 103</t>
+          <t>Русский язык - Room 206 - Teacher: Михаил С.К.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Физика - Room 110 - Teacher: Роман А.Д.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Geography - Room 316</t>
+          <t>География - Room 111 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Language - Room 206</t>
+          <t>Биология - Room 309 - Teacher: Светлана А.К.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Химия - Room 213 - Teacher: Оксана М.С.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>История - Room 114 - Teacher: Наталья Д.З.</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1760,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1494,6 +1794,16 @@
           <t>Lesson 5</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Lesson 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -1503,27 +1813,37 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Language - Room 200</t>
+          <t>Русский язык - Room 213 - Teacher: Александр И.Р.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Физическая культура - Room 109 - Teacher: Светлана А.К.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Language - Room 206</t>
+          <t>Русский язык - Room 213 - Teacher: Ольга В.С.</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Chemistry - Room 214</t>
+          <t>Литература - Room 210 - Teacher: Илья В.М.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Math - Room 100</t>
+          <t>Русский язык - Room 204 - Teacher: Екатерина А.П.</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Русский язык - Room 108 - Teacher: Михаил С.К.</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Иностранный язык - Room 208 - Teacher: Елена В.К.</t>
         </is>
       </c>
     </row>
@@ -1535,27 +1855,37 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Math - Room 100</t>
+          <t>География - Room 111 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Physics - Room 113</t>
+          <t>Математика - Room 108 - Teacher: Марина Г.Б.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Biology - Room 310</t>
+          <t>Информатика - Room 107 - Teacher: Алёна В.Л.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Math - Room 106</t>
+          <t>Математика - Room 109 - Teacher: Евгения О.П.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Math - Room 101</t>
+          <t>Физика - Room 113 - Teacher: Игорь В.Н.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Физика - Room 111 - Teacher: Роман А.Д.</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Обществознание - Room 212 - Teacher: Наталья Д.З.</t>
         </is>
       </c>
     </row>
@@ -1567,27 +1897,37 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Math - Room 108</t>
+          <t>Физика - Room 113 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Math - Room 107</t>
+          <t>Математика - Room 108 - Teacher: Константин В.Л.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>X - Room 0 - Teacher: X</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Chemistry - Room 212</t>
+          <t>Литература - Room 103 - Teacher: Петр И.С.</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Physics - Room 112</t>
+          <t>География - Room 109 - Teacher: Василий И.М.</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Физическая культура - Room 109 - Teacher: Светлана А.К.</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Биология - Room 310 - Teacher: Андрей П.С.</t>
         </is>
       </c>
     </row>
@@ -1599,27 +1939,37 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Language - Room 208</t>
+          <t>Химия - Room 212 - Teacher: Анастасия А.Ф.</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Geography - Room 316</t>
+          <t>Химия - Room 212 - Teacher: Оксана М.С.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>History - Room 318</t>
+          <t>История - Room 110 - Teacher: Наталья Д.З.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Biology - Room 309</t>
+          <t>Литература - Room 105 - Teacher: Петр И.С.</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Иностранный язык - Room 205 - Teacher: Юлия Н.В.</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>История - Room 110 - Teacher: Елена В.К.</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Информатика - Room 107 - Teacher: Алёна В.Л.</t>
         </is>
       </c>
     </row>
@@ -1631,27 +1981,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Language - Room 207</t>
+          <t>Математика - Room 104 - Teacher: Евгения О.П.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Language - Room 203</t>
+          <t>Математика - Room 108 - Teacher: Евгения О.П.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>X - Room 0</t>
+          <t>Информатика - Room 107 - Teacher: Игорь В.Н.</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Language - Room 203</t>
+          <t>Химия - Room 213 - Teacher: Оксана М.С.</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Math - Room 102</t>
+          <t>Обществознание - Room 213 - Teacher: Наталья Д.З.</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Математика - Room 109 - Teacher: Константин В.Л.</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Биология - Room 310 - Teacher: Андрей П.С.</t>
         </is>
       </c>
     </row>

</xml_diff>